<commit_message>
Création Excel Cost Model
</commit_message>
<xml_diff>
--- a/CR_Cost_Report/01_BOM/00_Cost_Report_Document/Ressources COST Model/Cost_v1.5.xlsx
+++ b/CR_Cost_Report/01_BOM/00_Cost_Report_Document/Ressources COST Model/Cost_v1.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\OneDrive\Documents\EPSA\Optipute\CR - Cost Report\CBOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33645\Documents\02-Etudes\2019-ECL\Trans Semestres\01-EPSA\03-Trans Saisons\Git\ELIZ-2021\CR_Cost_Report\01_BOM\00_Cost_Report_Document\Ressources COST Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CFAF20-9551-4064-BCC5-EC3023708C1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61025939-CD7B-41EB-A312-2A88CEA18A0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="667" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -27,15 +27,10 @@
     <sheet name="Conventionnal machinning" sheetId="15" r:id="rId12"/>
     <sheet name="Material" sheetId="2" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3029,161 +3024,197 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3209,39 +3240,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3306,9 +3304,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6521,7 +6516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -6552,29 +6547,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="260" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
       <c r="D1" s="48"/>
-      <c r="F1" s="229" t="s">
+      <c r="F1" s="254" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="230"/>
-      <c r="H1" s="230"/>
-      <c r="I1" s="230"/>
-      <c r="J1" s="231"/>
-      <c r="L1" s="232" t="s">
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="256"/>
+      <c r="L1" s="257" t="s">
         <v>209</v>
       </c>
-      <c r="M1" s="233"/>
-      <c r="N1" s="233"/>
-      <c r="O1" s="233"/>
-      <c r="P1" s="233"/>
-      <c r="Q1" s="233"/>
-      <c r="R1" s="233"/>
-      <c r="S1" s="234"/>
+      <c r="M1" s="258"/>
+      <c r="N1" s="258"/>
+      <c r="O1" s="258"/>
+      <c r="P1" s="258"/>
+      <c r="Q1" s="258"/>
+      <c r="R1" s="258"/>
+      <c r="S1" s="259"/>
     </row>
     <row r="2" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
@@ -6638,7 +6633,7 @@
         <f>'Manpower &amp; time'!D8</f>
         <v>21376</v>
       </c>
-      <c r="D3" s="251" t="s">
+      <c r="D3" s="271" t="s">
         <v>507</v>
       </c>
       <c r="F3" s="106" t="s">
@@ -6658,10 +6653,10 @@
         <f>H3/I3</f>
         <v>232</v>
       </c>
-      <c r="L3" s="237" t="s">
+      <c r="L3" s="235" t="s">
         <v>474</v>
       </c>
-      <c r="M3" s="268"/>
+      <c r="M3" s="236"/>
       <c r="N3" s="100" t="s">
         <v>208</v>
       </c>
@@ -6690,7 +6685,7 @@
         <f>'Manpower &amp; time'!D9</f>
         <v>39809</v>
       </c>
-      <c r="D4" s="252"/>
+      <c r="D4" s="272"/>
       <c r="F4" s="107"/>
       <c r="G4" s="101" t="s">
         <v>198</v>
@@ -6740,7 +6735,7 @@
         <f>'Manpower &amp; time'!D11</f>
         <v>69843</v>
       </c>
-      <c r="D5" s="252"/>
+      <c r="D5" s="272"/>
       <c r="F5" s="107"/>
       <c r="G5" s="101" t="s">
         <v>197</v>
@@ -6791,7 +6786,7 @@
         <f>'Manpower &amp; time'!D9</f>
         <v>39809</v>
       </c>
-      <c r="D6" s="253"/>
+      <c r="D6" s="273"/>
       <c r="F6" s="107"/>
       <c r="G6" s="101" t="s">
         <v>32</v>
@@ -7052,10 +7047,10 @@
         <f t="shared" si="0"/>
         <v>1999.4687999999999</v>
       </c>
-      <c r="L11" s="246" t="s">
+      <c r="L11" s="230" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="247"/>
+      <c r="M11" s="269"/>
       <c r="N11" s="100" t="s">
         <v>316</v>
       </c>
@@ -7378,7 +7373,7 @@
         <f t="shared" si="0"/>
         <v>64.320000000000007</v>
       </c>
-      <c r="L18" s="318" t="s">
+      <c r="L18" s="225" t="s">
         <v>244</v>
       </c>
       <c r="M18" s="140">
@@ -7407,10 +7402,10 @@
         <f t="shared" si="0"/>
         <v>277.54199999999997</v>
       </c>
-      <c r="L19" s="269" t="s">
+      <c r="L19" s="237" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="270"/>
+      <c r="M19" s="238"/>
       <c r="N19" s="100" t="s">
         <v>21</v>
       </c>
@@ -7957,10 +7952,10 @@
       <c r="N34" s="101" t="s">
         <v>448</v>
       </c>
-      <c r="O34" s="254" t="s">
+      <c r="O34" s="274" t="s">
         <v>214</v>
       </c>
-      <c r="P34" s="255" t="s">
+      <c r="P34" s="275" t="s">
         <v>447</v>
       </c>
       <c r="Q34" s="29">
@@ -7991,8 +7986,8 @@
       <c r="N35" s="101" t="s">
         <v>449</v>
       </c>
-      <c r="O35" s="254"/>
-      <c r="P35" s="255"/>
+      <c r="O35" s="274"/>
+      <c r="P35" s="275"/>
       <c r="Q35" s="29">
         <f>Welding!B23</f>
         <v>5.0185057685504804E-2</v>
@@ -8050,10 +8045,10 @@
         <f>H37/I37</f>
         <v>1874.5019999999997</v>
       </c>
-      <c r="L37" s="246" t="s">
+      <c r="L37" s="230" t="s">
         <v>389</v>
       </c>
-      <c r="M37" s="247"/>
+      <c r="M37" s="269"/>
       <c r="N37" s="100" t="s">
         <v>453</v>
       </c>
@@ -8144,13 +8139,13 @@
       </c>
     </row>
     <row r="40" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="239" t="s">
+      <c r="F40" s="263" t="s">
         <v>511</v>
       </c>
-      <c r="G40" s="240"/>
-      <c r="H40" s="240"/>
-      <c r="I40" s="240"/>
-      <c r="J40" s="241"/>
+      <c r="G40" s="264"/>
+      <c r="H40" s="264"/>
+      <c r="I40" s="264"/>
+      <c r="J40" s="265"/>
       <c r="L40" s="42" t="s">
         <v>226</v>
       </c>
@@ -8179,14 +8174,14 @@
       </c>
     </row>
     <row r="41" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F41" s="256" t="s">
+      <c r="F41" s="244" t="s">
         <v>309</v>
       </c>
-      <c r="G41" s="244" t="s">
+      <c r="G41" s="267" t="s">
         <v>470</v>
       </c>
-      <c r="H41" s="244"/>
-      <c r="I41" s="245"/>
+      <c r="H41" s="267"/>
+      <c r="I41" s="268"/>
       <c r="J41" s="87">
         <f>SUM(J3:J38)*1.05</f>
         <v>129206.09501598139</v>
@@ -8215,12 +8210,12 @@
       <c r="S41" s="141"/>
     </row>
     <row r="42" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="257"/>
-      <c r="G42" s="242" t="s">
+      <c r="F42" s="245"/>
+      <c r="G42" s="266" t="s">
         <v>271</v>
       </c>
-      <c r="H42" s="242"/>
-      <c r="I42" s="243"/>
+      <c r="H42" s="266"/>
+      <c r="I42" s="252"/>
       <c r="J42" s="88">
         <f>J41/SUM('Manpower &amp; time'!C32:J32)</f>
         <v>11.853030729824322</v>
@@ -8247,87 +8242,87 @@
       <c r="S42" s="73"/>
     </row>
     <row r="43" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="258" t="s">
+      <c r="F43" s="246" t="s">
         <v>310</v>
       </c>
-      <c r="G43" s="245" t="s">
+      <c r="G43" s="268" t="s">
         <v>311</v>
       </c>
-      <c r="H43" s="248"/>
-      <c r="I43" s="248"/>
+      <c r="H43" s="270"/>
+      <c r="I43" s="270"/>
       <c r="J43" s="89">
         <f>'Manpower &amp; time'!H8</f>
         <v>12.723809523809523</v>
       </c>
     </row>
     <row r="44" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F44" s="259"/>
-      <c r="G44" s="249" t="s">
+      <c r="F44" s="247"/>
+      <c r="G44" s="242" t="s">
         <v>322</v>
       </c>
-      <c r="H44" s="250"/>
-      <c r="I44" s="250"/>
+      <c r="H44" s="243"/>
+      <c r="I44" s="243"/>
       <c r="J44" s="90">
         <f>'Manpower &amp; time'!H9</f>
         <v>23.695833333333333</v>
       </c>
-      <c r="L44" s="261" t="s">
+      <c r="L44" s="249" t="s">
         <v>512</v>
       </c>
-      <c r="M44" s="262"/>
-      <c r="N44" s="262"/>
-      <c r="O44" s="262"/>
-      <c r="P44" s="262"/>
-      <c r="Q44" s="262"/>
-      <c r="R44" s="263"/>
+      <c r="M44" s="250"/>
+      <c r="N44" s="250"/>
+      <c r="O44" s="250"/>
+      <c r="P44" s="250"/>
+      <c r="Q44" s="250"/>
+      <c r="R44" s="251"/>
     </row>
     <row r="45" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="F45" s="259"/>
-      <c r="G45" s="249" t="s">
+      <c r="F45" s="247"/>
+      <c r="G45" s="242" t="s">
         <v>464</v>
       </c>
-      <c r="H45" s="250"/>
-      <c r="I45" s="250"/>
+      <c r="H45" s="243"/>
+      <c r="I45" s="243"/>
       <c r="J45" s="90">
         <f>'Manpower &amp; time'!H10</f>
         <v>29.85654761904761</v>
       </c>
-      <c r="L45" s="237" t="s">
+      <c r="L45" s="235" t="s">
         <v>474</v>
       </c>
-      <c r="M45" s="238"/>
-      <c r="N45" s="265" t="s">
+      <c r="M45" s="262"/>
+      <c r="N45" s="232" t="s">
         <v>280</v>
       </c>
-      <c r="O45" s="265"/>
-      <c r="P45" s="265"/>
-      <c r="Q45" s="265"/>
+      <c r="O45" s="232"/>
+      <c r="P45" s="232"/>
+      <c r="Q45" s="232"/>
       <c r="R45" s="77">
         <f>SUM(S3:S6)+S9</f>
         <v>17591.025600000001</v>
       </c>
     </row>
     <row r="46" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F46" s="260"/>
-      <c r="G46" s="243" t="s">
+      <c r="F46" s="248"/>
+      <c r="G46" s="252" t="s">
         <v>312</v>
       </c>
-      <c r="H46" s="264"/>
-      <c r="I46" s="264"/>
+      <c r="H46" s="253"/>
+      <c r="I46" s="253"/>
       <c r="J46" s="91">
         <f>'Manpower &amp; time'!H11</f>
         <v>41.573214285714279</v>
       </c>
-      <c r="L46" s="274" t="s">
+      <c r="L46" s="227" t="s">
         <v>478</v>
       </c>
-      <c r="M46" s="275"/>
-      <c r="N46" s="225" t="s">
+      <c r="M46" s="228"/>
+      <c r="N46" s="226" t="s">
         <v>281</v>
       </c>
-      <c r="O46" s="225"/>
-      <c r="P46" s="225"/>
-      <c r="Q46" s="225"/>
+      <c r="O46" s="226"/>
+      <c r="P46" s="226"/>
+      <c r="Q46" s="226"/>
       <c r="R46" s="78">
         <f>R45/(M5*C7*C8)+J42</f>
         <v>25.63046306065139</v>
@@ -8341,12 +8336,12 @@
       <c r="M47" s="38">
         <v>2.5</v>
       </c>
-      <c r="N47" s="225" t="s">
+      <c r="N47" s="226" t="s">
         <v>282</v>
       </c>
-      <c r="O47" s="225"/>
-      <c r="P47" s="225"/>
-      <c r="Q47" s="225"/>
+      <c r="O47" s="226"/>
+      <c r="P47" s="226"/>
+      <c r="Q47" s="226"/>
       <c r="R47" s="78">
         <f>R46+Q8+Q7</f>
         <v>47.03359906065139</v>
@@ -8360,10 +8355,10 @@
       <c r="M48" s="38">
         <v>0.5</v>
       </c>
-      <c r="N48" s="225"/>
-      <c r="O48" s="225"/>
-      <c r="P48" s="225"/>
-      <c r="Q48" s="225"/>
+      <c r="N48" s="226"/>
+      <c r="O48" s="226"/>
+      <c r="P48" s="226"/>
+      <c r="Q48" s="226"/>
       <c r="R48" s="79"/>
     </row>
     <row r="49" spans="6:18" x14ac:dyDescent="0.25">
@@ -8371,12 +8366,12 @@
       <c r="J49" s="14"/>
       <c r="L49" s="21"/>
       <c r="M49" s="22"/>
-      <c r="N49" s="225" t="s">
+      <c r="N49" s="226" t="s">
         <v>267</v>
       </c>
-      <c r="O49" s="225"/>
-      <c r="P49" s="225"/>
-      <c r="Q49" s="225"/>
+      <c r="O49" s="226"/>
+      <c r="P49" s="226"/>
+      <c r="Q49" s="226"/>
       <c r="R49" s="80">
         <f>('Manpower &amp; time'!H8+R47)*M7/60</f>
         <v>9.9595680974101528E-5</v>
@@ -8387,12 +8382,12 @@
       <c r="J50" s="14"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22"/>
-      <c r="N50" s="225" t="s">
+      <c r="N50" s="226" t="s">
         <v>469</v>
       </c>
-      <c r="O50" s="225"/>
-      <c r="P50" s="225"/>
-      <c r="Q50" s="225"/>
+      <c r="O50" s="226"/>
+      <c r="P50" s="226"/>
+      <c r="Q50" s="226"/>
       <c r="R50" s="81">
         <f>('Manpower &amp; time'!H8)*M7/60/R49</f>
         <v>0.21292438586632709</v>
@@ -8403,21 +8398,21 @@
       <c r="J51" s="14"/>
       <c r="L51" s="21"/>
       <c r="M51" s="22"/>
-      <c r="N51" s="225"/>
-      <c r="O51" s="225"/>
-      <c r="P51" s="225"/>
-      <c r="Q51" s="225"/>
+      <c r="N51" s="226"/>
+      <c r="O51" s="226"/>
+      <c r="P51" s="226"/>
+      <c r="Q51" s="226"/>
       <c r="R51" s="80"/>
     </row>
     <row r="52" spans="6:18" x14ac:dyDescent="0.25">
       <c r="L52" s="21"/>
       <c r="M52" s="22"/>
-      <c r="N52" s="225" t="s">
+      <c r="N52" s="226" t="s">
         <v>270</v>
       </c>
-      <c r="O52" s="225"/>
-      <c r="P52" s="225"/>
-      <c r="Q52" s="225"/>
+      <c r="O52" s="226"/>
+      <c r="P52" s="226"/>
+      <c r="Q52" s="226"/>
       <c r="R52" s="80">
         <f>('Manpower &amp; time'!H8+J42)*M8/60</f>
         <v>2.0480700211361539E-5</v>
@@ -8427,12 +8422,12 @@
       <c r="J53" s="8"/>
       <c r="L53" s="21"/>
       <c r="M53" s="22"/>
-      <c r="N53" s="225" t="s">
+      <c r="N53" s="226" t="s">
         <v>268</v>
       </c>
-      <c r="O53" s="225"/>
-      <c r="P53" s="225"/>
-      <c r="Q53" s="225"/>
+      <c r="O53" s="226"/>
+      <c r="P53" s="226"/>
+      <c r="Q53" s="226"/>
       <c r="R53" s="80">
         <f>('Manpower &amp; time'!H9+J42)*M8/60</f>
         <v>2.9624053385964713E-5</v>
@@ -8442,12 +8437,12 @@
       <c r="J54" s="7"/>
       <c r="L54" s="21"/>
       <c r="M54" s="22"/>
-      <c r="N54" s="225" t="s">
+      <c r="N54" s="226" t="s">
         <v>269</v>
       </c>
-      <c r="O54" s="225"/>
-      <c r="P54" s="225"/>
-      <c r="Q54" s="225"/>
+      <c r="O54" s="226"/>
+      <c r="P54" s="226"/>
+      <c r="Q54" s="226"/>
       <c r="R54" s="80">
         <f>('Manpower &amp; time'!H11+J42)*M8/60</f>
         <v>4.4521870846282167E-5</v>
@@ -8457,12 +8452,12 @@
       <c r="J55" s="7"/>
       <c r="L55" s="21"/>
       <c r="M55" s="22"/>
-      <c r="N55" s="225" t="s">
+      <c r="N55" s="226" t="s">
         <v>313</v>
       </c>
-      <c r="O55" s="225"/>
-      <c r="P55" s="225"/>
-      <c r="Q55" s="225"/>
+      <c r="O55" s="226"/>
+      <c r="P55" s="226"/>
+      <c r="Q55" s="226"/>
       <c r="R55" s="80">
         <f>('Manpower &amp; time'!H8+J42)*M$9/60</f>
         <v>1.6384560169089233E-5</v>
@@ -8472,12 +8467,12 @@
       <c r="J56" s="7"/>
       <c r="L56" s="21"/>
       <c r="M56" s="22"/>
-      <c r="N56" s="225" t="s">
+      <c r="N56" s="226" t="s">
         <v>314</v>
       </c>
-      <c r="O56" s="225"/>
-      <c r="P56" s="225"/>
-      <c r="Q56" s="225"/>
+      <c r="O56" s="226"/>
+      <c r="P56" s="226"/>
+      <c r="Q56" s="226"/>
       <c r="R56" s="80">
         <f>('Manpower &amp; time'!H9+J42)*M$9/60</f>
         <v>2.3699242708771769E-5</v>
@@ -8487,12 +8482,12 @@
       <c r="J57" s="5"/>
       <c r="L57" s="21"/>
       <c r="M57" s="22"/>
-      <c r="N57" s="225" t="s">
+      <c r="N57" s="226" t="s">
         <v>315</v>
       </c>
-      <c r="O57" s="225"/>
-      <c r="P57" s="225"/>
-      <c r="Q57" s="225"/>
+      <c r="O57" s="226"/>
+      <c r="P57" s="226"/>
+      <c r="Q57" s="226"/>
       <c r="R57" s="80">
         <f>('Manpower &amp; time'!H11+J42)*M$9/60</f>
         <v>3.5617496677025735E-5</v>
@@ -8501,44 +8496,44 @@
     <row r="58" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L58" s="23"/>
       <c r="M58" s="24"/>
-      <c r="N58" s="226" t="s">
+      <c r="N58" s="229" t="s">
         <v>279</v>
       </c>
-      <c r="O58" s="226"/>
-      <c r="P58" s="226"/>
-      <c r="Q58" s="226"/>
+      <c r="O58" s="229"/>
+      <c r="P58" s="229"/>
+      <c r="Q58" s="229"/>
       <c r="R58" s="82">
         <f>('Manpower &amp; time'!H8+R46)*(M10+M6)/60</f>
         <v>15.980946910192047</v>
       </c>
     </row>
     <row r="59" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="L59" s="246" t="s">
+      <c r="L59" s="230" t="s">
         <v>18</v>
       </c>
-      <c r="M59" s="276"/>
-      <c r="N59" s="265" t="s">
+      <c r="M59" s="231"/>
+      <c r="N59" s="232" t="s">
         <v>280</v>
       </c>
-      <c r="O59" s="265"/>
-      <c r="P59" s="265"/>
-      <c r="Q59" s="265"/>
+      <c r="O59" s="232"/>
+      <c r="P59" s="232"/>
+      <c r="Q59" s="232"/>
       <c r="R59" s="77">
         <f>SUM(S11:S14)+S17</f>
         <v>23026.025600000001</v>
       </c>
     </row>
     <row r="60" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="L60" s="272" t="s">
+      <c r="L60" s="240" t="s">
         <v>478</v>
       </c>
-      <c r="M60" s="273"/>
-      <c r="N60" s="225" t="s">
+      <c r="M60" s="241"/>
+      <c r="N60" s="226" t="s">
         <v>281</v>
       </c>
-      <c r="O60" s="225"/>
-      <c r="P60" s="225"/>
-      <c r="Q60" s="225"/>
+      <c r="O60" s="226"/>
+      <c r="P60" s="226"/>
+      <c r="Q60" s="226"/>
       <c r="R60" s="78">
         <f>R59/(M13*C7*C8)+J42</f>
         <v>29.887198649623823</v>
@@ -8552,12 +8547,12 @@
       <c r="M61" s="40">
         <v>2.5</v>
       </c>
-      <c r="N61" s="225" t="s">
+      <c r="N61" s="226" t="s">
         <v>282</v>
       </c>
-      <c r="O61" s="225"/>
-      <c r="P61" s="225"/>
-      <c r="Q61" s="225"/>
+      <c r="O61" s="226"/>
+      <c r="P61" s="226"/>
+      <c r="Q61" s="226"/>
       <c r="R61" s="78">
         <f>R60+Q16+Q15</f>
         <v>41.753870649623828</v>
@@ -8570,22 +8565,22 @@
       <c r="M62" s="40">
         <v>0.5</v>
       </c>
-      <c r="N62" s="225"/>
-      <c r="O62" s="225"/>
-      <c r="P62" s="225"/>
-      <c r="Q62" s="225"/>
+      <c r="N62" s="226"/>
+      <c r="O62" s="226"/>
+      <c r="P62" s="226"/>
+      <c r="Q62" s="226"/>
       <c r="R62" s="79"/>
     </row>
     <row r="63" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F63" s="11"/>
       <c r="L63" s="17"/>
       <c r="M63" s="18"/>
-      <c r="N63" s="225" t="s">
+      <c r="N63" s="226" t="s">
         <v>267</v>
       </c>
-      <c r="O63" s="225"/>
-      <c r="P63" s="225"/>
-      <c r="Q63" s="225"/>
+      <c r="O63" s="226"/>
+      <c r="P63" s="226"/>
+      <c r="Q63" s="226"/>
       <c r="R63" s="80">
         <f>(J43+R61)*M15/60</f>
         <v>9.0796133622388927E-5</v>
@@ -8594,12 +8589,12 @@
     <row r="64" spans="6:18" x14ac:dyDescent="0.25">
       <c r="L64" s="17"/>
       <c r="M64" s="18"/>
-      <c r="N64" s="225" t="s">
+      <c r="N64" s="226" t="s">
         <v>469</v>
       </c>
-      <c r="O64" s="225"/>
-      <c r="P64" s="225"/>
-      <c r="Q64" s="225"/>
+      <c r="O64" s="226"/>
+      <c r="P64" s="226"/>
+      <c r="Q64" s="226"/>
       <c r="R64" s="81">
         <f>(J43)*M15/60/R63</f>
         <v>0.23356004667053407</v>
@@ -8608,21 +8603,21 @@
     <row r="65" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L65" s="17"/>
       <c r="M65" s="18"/>
-      <c r="N65" s="225"/>
-      <c r="O65" s="225"/>
-      <c r="P65" s="225"/>
-      <c r="Q65" s="225"/>
+      <c r="N65" s="226"/>
+      <c r="O65" s="226"/>
+      <c r="P65" s="226"/>
+      <c r="Q65" s="226"/>
       <c r="R65" s="80"/>
     </row>
     <row r="66" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L66" s="17"/>
       <c r="M66" s="18"/>
-      <c r="N66" s="225" t="s">
+      <c r="N66" s="226" t="s">
         <v>270</v>
       </c>
-      <c r="O66" s="225"/>
-      <c r="P66" s="225"/>
-      <c r="Q66" s="225"/>
+      <c r="O66" s="226"/>
+      <c r="P66" s="226"/>
+      <c r="Q66" s="226"/>
       <c r="R66" s="80">
         <f>(J43+J42)*M$16/60</f>
         <v>2.0480700211361539E-5</v>
@@ -8631,12 +8626,12 @@
     <row r="67" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L67" s="17"/>
       <c r="M67" s="18"/>
-      <c r="N67" s="225" t="s">
+      <c r="N67" s="226" t="s">
         <v>268</v>
       </c>
-      <c r="O67" s="225"/>
-      <c r="P67" s="225"/>
-      <c r="Q67" s="225"/>
+      <c r="O67" s="226"/>
+      <c r="P67" s="226"/>
+      <c r="Q67" s="226"/>
       <c r="R67" s="80">
         <f>(J44+J42)*M$16/60</f>
         <v>2.9624053385964713E-5</v>
@@ -8645,12 +8640,12 @@
     <row r="68" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L68" s="17"/>
       <c r="M68" s="18"/>
-      <c r="N68" s="225" t="s">
+      <c r="N68" s="226" t="s">
         <v>269</v>
       </c>
-      <c r="O68" s="225"/>
-      <c r="P68" s="225"/>
-      <c r="Q68" s="225"/>
+      <c r="O68" s="226"/>
+      <c r="P68" s="226"/>
+      <c r="Q68" s="226"/>
       <c r="R68" s="80">
         <f>(J46+J42)*M$16/60</f>
         <v>4.4521870846282167E-5</v>
@@ -8659,12 +8654,12 @@
     <row r="69" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L69" s="17"/>
       <c r="M69" s="18"/>
-      <c r="N69" s="225" t="s">
+      <c r="N69" s="226" t="s">
         <v>313</v>
       </c>
-      <c r="O69" s="225"/>
-      <c r="P69" s="225"/>
-      <c r="Q69" s="225"/>
+      <c r="O69" s="226"/>
+      <c r="P69" s="226"/>
+      <c r="Q69" s="226"/>
       <c r="R69" s="80">
         <f>(J43+J42)*M$17/60</f>
         <v>1.6384560169089233E-5</v>
@@ -8673,12 +8668,12 @@
     <row r="70" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L70" s="17"/>
       <c r="M70" s="18"/>
-      <c r="N70" s="225" t="s">
+      <c r="N70" s="226" t="s">
         <v>314</v>
       </c>
-      <c r="O70" s="225"/>
-      <c r="P70" s="225"/>
-      <c r="Q70" s="225"/>
+      <c r="O70" s="226"/>
+      <c r="P70" s="226"/>
+      <c r="Q70" s="226"/>
       <c r="R70" s="80">
         <f>(J44+J42)*M$17/60</f>
         <v>2.3699242708771769E-5</v>
@@ -8687,12 +8682,12 @@
     <row r="71" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L71" s="17"/>
       <c r="M71" s="18"/>
-      <c r="N71" s="225" t="s">
+      <c r="N71" s="226" t="s">
         <v>315</v>
       </c>
-      <c r="O71" s="225"/>
-      <c r="P71" s="225"/>
-      <c r="Q71" s="225"/>
+      <c r="O71" s="226"/>
+      <c r="P71" s="226"/>
+      <c r="Q71" s="226"/>
       <c r="R71" s="80">
         <f>(J46+J42)*M$17/60</f>
         <v>3.5617496677025735E-5</v>
@@ -8701,44 +8696,44 @@
     <row r="72" spans="12:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L72" s="17"/>
       <c r="M72" s="18"/>
-      <c r="N72" s="227" t="s">
+      <c r="N72" s="276" t="s">
         <v>279</v>
       </c>
-      <c r="O72" s="227"/>
-      <c r="P72" s="227"/>
-      <c r="Q72" s="227"/>
+      <c r="O72" s="276"/>
+      <c r="P72" s="276"/>
+      <c r="Q72" s="276"/>
       <c r="R72" s="154">
         <f>(J43+R60)*(M14+M18)/60</f>
         <v>14.203669391144448</v>
       </c>
     </row>
     <row r="73" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L73" s="269" t="s">
+      <c r="L73" s="237" t="s">
         <v>403</v>
       </c>
-      <c r="M73" s="271"/>
-      <c r="N73" s="265" t="s">
+      <c r="M73" s="239"/>
+      <c r="N73" s="232" t="s">
         <v>280</v>
       </c>
-      <c r="O73" s="265"/>
-      <c r="P73" s="265"/>
-      <c r="Q73" s="265"/>
+      <c r="O73" s="232"/>
+      <c r="P73" s="232"/>
+      <c r="Q73" s="232"/>
       <c r="R73" s="77">
         <f>S19+S20</f>
         <v>27751.54031372827</v>
       </c>
     </row>
     <row r="74" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L74" s="266" t="s">
+      <c r="L74" s="233" t="s">
         <v>479</v>
       </c>
-      <c r="M74" s="267"/>
-      <c r="N74" s="225" t="s">
+      <c r="M74" s="234"/>
+      <c r="N74" s="226" t="s">
         <v>281</v>
       </c>
-      <c r="O74" s="225"/>
-      <c r="P74" s="225"/>
-      <c r="Q74" s="225"/>
+      <c r="O74" s="226"/>
+      <c r="P74" s="226"/>
+      <c r="Q74" s="226"/>
       <c r="R74" s="78">
         <f>R73/(M21*C7*C8)+J42</f>
         <v>36.693292378345866</v>
@@ -8752,114 +8747,114 @@
         <f>'Laser cutter'!J14</f>
         <v>0.71739130434782605</v>
       </c>
-      <c r="N75" s="225" t="s">
+      <c r="N75" s="226" t="s">
         <v>282</v>
       </c>
-      <c r="O75" s="225"/>
-      <c r="P75" s="225"/>
-      <c r="Q75" s="225"/>
+      <c r="O75" s="226"/>
+      <c r="P75" s="226"/>
+      <c r="Q75" s="226"/>
       <c r="R75" s="78">
         <f>R74+Q21+Q22</f>
         <v>42.235892378345866</v>
       </c>
     </row>
     <row r="76" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L76" s="266"/>
-      <c r="M76" s="267"/>
-      <c r="N76" s="225"/>
-      <c r="O76" s="225"/>
-      <c r="P76" s="225"/>
-      <c r="Q76" s="225"/>
+      <c r="L76" s="233"/>
+      <c r="M76" s="234"/>
+      <c r="N76" s="226"/>
+      <c r="O76" s="226"/>
+      <c r="P76" s="226"/>
+      <c r="Q76" s="226"/>
       <c r="R76" s="79"/>
     </row>
     <row r="77" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L77" s="266"/>
-      <c r="M77" s="267"/>
-      <c r="N77" s="225" t="s">
+      <c r="L77" s="233"/>
+      <c r="M77" s="234"/>
+      <c r="N77" s="226" t="s">
         <v>404</v>
       </c>
-      <c r="O77" s="225"/>
-      <c r="P77" s="225"/>
-      <c r="Q77" s="225"/>
+      <c r="O77" s="226"/>
+      <c r="P77" s="226"/>
+      <c r="Q77" s="226"/>
       <c r="R77" s="80">
         <f>(J43*0.4+R75)*M23/60</f>
         <v>3.6282819077366752E-4</v>
       </c>
     </row>
     <row r="78" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L78" s="266"/>
-      <c r="M78" s="267"/>
-      <c r="N78" s="225" t="s">
+      <c r="L78" s="233"/>
+      <c r="M78" s="234"/>
+      <c r="N78" s="226" t="s">
         <v>469</v>
       </c>
-      <c r="O78" s="225"/>
-      <c r="P78" s="225"/>
-      <c r="Q78" s="225"/>
+      <c r="O78" s="226"/>
+      <c r="P78" s="226"/>
+      <c r="Q78" s="226"/>
       <c r="R78" s="81">
         <f>(J43)*M23/60/R77</f>
         <v>0.26885784740485508</v>
       </c>
     </row>
     <row r="79" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L79" s="266"/>
-      <c r="M79" s="267"/>
-      <c r="N79" s="225"/>
-      <c r="O79" s="225"/>
-      <c r="P79" s="225"/>
-      <c r="Q79" s="225"/>
+      <c r="L79" s="233"/>
+      <c r="M79" s="234"/>
+      <c r="N79" s="226"/>
+      <c r="O79" s="226"/>
+      <c r="P79" s="226"/>
+      <c r="Q79" s="226"/>
       <c r="R79" s="141"/>
     </row>
     <row r="80" spans="12:18" x14ac:dyDescent="0.25">
-      <c r="L80" s="266"/>
-      <c r="M80" s="267"/>
-      <c r="N80" s="225" t="s">
+      <c r="L80" s="233"/>
+      <c r="M80" s="234"/>
+      <c r="N80" s="226" t="s">
         <v>501</v>
       </c>
-      <c r="O80" s="225"/>
-      <c r="P80" s="225"/>
-      <c r="Q80" s="225"/>
+      <c r="O80" s="226"/>
+      <c r="P80" s="226"/>
+      <c r="Q80" s="226"/>
       <c r="R80" s="153">
         <f>(J43+J42)*M24/60</f>
         <v>0.61442100634084618</v>
       </c>
     </row>
     <row r="81" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L81" s="266"/>
-      <c r="M81" s="267"/>
-      <c r="N81" s="225" t="s">
+      <c r="L81" s="233"/>
+      <c r="M81" s="234"/>
+      <c r="N81" s="226" t="s">
         <v>502</v>
       </c>
-      <c r="O81" s="225"/>
-      <c r="P81" s="225"/>
-      <c r="Q81" s="225"/>
+      <c r="O81" s="226"/>
+      <c r="P81" s="226"/>
+      <c r="Q81" s="226"/>
       <c r="R81" s="153">
         <f>(J44+J42)*M24/60</f>
         <v>0.88872160157894131</v>
       </c>
     </row>
     <row r="82" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L82" s="266"/>
-      <c r="M82" s="267"/>
-      <c r="N82" s="225" t="s">
+      <c r="L82" s="233"/>
+      <c r="M82" s="234"/>
+      <c r="N82" s="226" t="s">
         <v>503</v>
       </c>
-      <c r="O82" s="225"/>
-      <c r="P82" s="225"/>
-      <c r="Q82" s="225"/>
+      <c r="O82" s="226"/>
+      <c r="P82" s="226"/>
+      <c r="Q82" s="226"/>
       <c r="R82" s="153">
         <f>(J43+J42)*M25/60</f>
         <v>0.40961400422723077</v>
       </c>
     </row>
     <row r="83" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L83" s="266"/>
-      <c r="M83" s="267"/>
-      <c r="N83" s="225" t="s">
+      <c r="L83" s="233"/>
+      <c r="M83" s="234"/>
+      <c r="N83" s="226" t="s">
         <v>504</v>
       </c>
-      <c r="O83" s="225"/>
-      <c r="P83" s="225"/>
-      <c r="Q83" s="225"/>
+      <c r="O83" s="226"/>
+      <c r="P83" s="226"/>
+      <c r="Q83" s="226"/>
       <c r="R83" s="153">
         <f>(J44+J42)*M$25/60</f>
         <v>0.59248106771929421</v>
@@ -8868,28 +8863,28 @@
     <row r="84" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L84" s="32"/>
       <c r="M84" s="33"/>
-      <c r="N84" s="226" t="s">
+      <c r="N84" s="229" t="s">
         <v>279</v>
       </c>
-      <c r="O84" s="226"/>
-      <c r="P84" s="226"/>
-      <c r="Q84" s="226"/>
+      <c r="O84" s="229"/>
+      <c r="P84" s="229"/>
+      <c r="Q84" s="229"/>
       <c r="R84" s="82">
         <f>(J43+R74)*(M26+M22)/60</f>
         <v>10.707038745467001</v>
       </c>
     </row>
     <row r="85" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L85" s="274" t="s">
+      <c r="L85" s="227" t="s">
         <v>24</v>
       </c>
-      <c r="M85" s="275"/>
-      <c r="N85" s="228" t="s">
+      <c r="M85" s="228"/>
+      <c r="N85" s="277" t="s">
         <v>280</v>
       </c>
-      <c r="O85" s="228"/>
-      <c r="P85" s="228"/>
-      <c r="Q85" s="228"/>
+      <c r="O85" s="277"/>
+      <c r="P85" s="277"/>
+      <c r="Q85" s="277"/>
       <c r="R85" s="155">
         <f>SUM(S27:S32)</f>
         <v>2176.9659999999999</v>
@@ -8898,12 +8893,12 @@
     <row r="86" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L86" s="44"/>
       <c r="M86" s="45"/>
-      <c r="N86" s="225" t="s">
+      <c r="N86" s="226" t="s">
         <v>281</v>
       </c>
-      <c r="O86" s="225"/>
-      <c r="P86" s="225"/>
-      <c r="Q86" s="225"/>
+      <c r="O86" s="226"/>
+      <c r="P86" s="226"/>
+      <c r="Q86" s="226"/>
       <c r="R86" s="97">
         <f>R85/(M29*C7*C8)+J42</f>
         <v>13.558047960400764</v>
@@ -8913,12 +8908,12 @@
     <row r="87" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L87" s="21"/>
       <c r="M87" s="22"/>
-      <c r="N87" s="225" t="s">
+      <c r="N87" s="226" t="s">
         <v>282</v>
       </c>
-      <c r="O87" s="225"/>
-      <c r="P87" s="225"/>
-      <c r="Q87" s="225"/>
+      <c r="O87" s="226"/>
+      <c r="P87" s="226"/>
+      <c r="Q87" s="226"/>
       <c r="R87" s="97">
         <f>R86+Q33</f>
         <v>13.655922960400764</v>
@@ -8927,21 +8922,21 @@
     <row r="88" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L88" s="21"/>
       <c r="M88" s="22"/>
-      <c r="N88" s="225"/>
-      <c r="O88" s="225"/>
-      <c r="P88" s="225"/>
-      <c r="Q88" s="225"/>
+      <c r="N88" s="226"/>
+      <c r="O88" s="226"/>
+      <c r="P88" s="226"/>
+      <c r="Q88" s="226"/>
       <c r="R88" s="141"/>
     </row>
     <row r="89" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L89" s="21"/>
       <c r="M89" s="22"/>
-      <c r="N89" s="225" t="s">
+      <c r="N89" s="226" t="s">
         <v>451</v>
       </c>
-      <c r="O89" s="225"/>
-      <c r="P89" s="225"/>
-      <c r="Q89" s="225"/>
+      <c r="O89" s="226"/>
+      <c r="P89" s="226"/>
+      <c r="Q89" s="226"/>
       <c r="R89" s="61">
         <f>Q34+Q36+(R87+J45)*M30/60</f>
         <v>116.28085496788751</v>
@@ -8950,12 +8945,12 @@
     <row r="90" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L90" s="21"/>
       <c r="M90" s="22"/>
-      <c r="N90" s="225" t="s">
+      <c r="N90" s="226" t="s">
         <v>452</v>
       </c>
-      <c r="O90" s="225"/>
-      <c r="P90" s="225"/>
-      <c r="Q90" s="225"/>
+      <c r="O90" s="226"/>
+      <c r="P90" s="226"/>
+      <c r="Q90" s="226"/>
       <c r="R90" s="97">
         <f>Q35+Q36+(R87+J45)*M30/60</f>
         <v>116.24579290891785</v>
@@ -8964,23 +8959,23 @@
     <row r="91" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L91" s="23"/>
       <c r="M91" s="24"/>
-      <c r="N91" s="226"/>
-      <c r="O91" s="226"/>
-      <c r="P91" s="226"/>
-      <c r="Q91" s="226"/>
+      <c r="N91" s="229"/>
+      <c r="O91" s="229"/>
+      <c r="P91" s="229"/>
+      <c r="Q91" s="229"/>
       <c r="R91" s="73"/>
     </row>
     <row r="92" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L92" s="246" t="s">
+      <c r="L92" s="230" t="s">
         <v>389</v>
       </c>
-      <c r="M92" s="276"/>
-      <c r="N92" s="265" t="s">
+      <c r="M92" s="231"/>
+      <c r="N92" s="232" t="s">
         <v>280</v>
       </c>
-      <c r="O92" s="265"/>
-      <c r="P92" s="265"/>
-      <c r="Q92" s="265"/>
+      <c r="O92" s="232"/>
+      <c r="P92" s="232"/>
+      <c r="Q92" s="232"/>
       <c r="R92" s="77">
         <f>SUM(S37:S40)</f>
         <v>4775</v>
@@ -8989,12 +8984,12 @@
     <row r="93" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L93" s="42"/>
       <c r="M93" s="43"/>
-      <c r="N93" s="225" t="s">
+      <c r="N93" s="226" t="s">
         <v>281</v>
       </c>
-      <c r="O93" s="225"/>
-      <c r="P93" s="225"/>
-      <c r="Q93" s="225"/>
+      <c r="O93" s="226"/>
+      <c r="P93" s="226"/>
+      <c r="Q93" s="226"/>
       <c r="R93" s="78">
         <f>R92/(M39*C7*C8)+J42</f>
         <v>18.652700358441319</v>
@@ -9003,12 +8998,12 @@
     <row r="94" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L94" s="17"/>
       <c r="M94" s="18"/>
-      <c r="N94" s="225" t="s">
+      <c r="N94" s="226" t="s">
         <v>282</v>
       </c>
-      <c r="O94" s="225"/>
-      <c r="P94" s="225"/>
-      <c r="Q94" s="225"/>
+      <c r="O94" s="226"/>
+      <c r="P94" s="226"/>
+      <c r="Q94" s="226"/>
       <c r="R94" s="78">
         <f>R93+Q42+Q41</f>
         <v>29.028540358441319</v>
@@ -9017,21 +9012,21 @@
     <row r="95" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L95" s="17"/>
       <c r="M95" s="18"/>
-      <c r="N95" s="225"/>
-      <c r="O95" s="225"/>
-      <c r="P95" s="225"/>
-      <c r="Q95" s="225"/>
+      <c r="N95" s="226"/>
+      <c r="O95" s="226"/>
+      <c r="P95" s="226"/>
+      <c r="Q95" s="226"/>
       <c r="R95" s="79"/>
     </row>
     <row r="96" spans="12:19" x14ac:dyDescent="0.25">
       <c r="L96" s="17"/>
       <c r="M96" s="18"/>
-      <c r="N96" s="225" t="s">
+      <c r="N96" s="226" t="s">
         <v>267</v>
       </c>
-      <c r="O96" s="225"/>
-      <c r="P96" s="225"/>
-      <c r="Q96" s="225"/>
+      <c r="O96" s="226"/>
+      <c r="P96" s="226"/>
+      <c r="Q96" s="226"/>
       <c r="R96" s="80">
         <f>(J43+R94)*M41/60</f>
         <v>2.0876174941125418E-4</v>
@@ -9040,12 +9035,12 @@
     <row r="97" spans="12:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L97" s="19"/>
       <c r="M97" s="20"/>
-      <c r="N97" s="226" t="s">
+      <c r="N97" s="229" t="s">
         <v>279</v>
       </c>
-      <c r="O97" s="226"/>
-      <c r="P97" s="226"/>
-      <c r="Q97" s="226"/>
+      <c r="O97" s="229"/>
+      <c r="P97" s="229"/>
+      <c r="Q97" s="229"/>
       <c r="R97" s="82">
         <f>(J43+R93)*(M40+M42)/60</f>
         <v>7.8441274705627109</v>
@@ -9054,65 +9049,19 @@
     <row r="118" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="N94:Q94"/>
-    <mergeCell ref="N95:Q95"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N87:Q87"/>
-    <mergeCell ref="N88:Q88"/>
-    <mergeCell ref="N83:Q83"/>
-    <mergeCell ref="N84:Q84"/>
-    <mergeCell ref="L92:M92"/>
-    <mergeCell ref="N92:Q92"/>
-    <mergeCell ref="N93:Q93"/>
-    <mergeCell ref="L80:M80"/>
-    <mergeCell ref="L81:M81"/>
-    <mergeCell ref="L82:M82"/>
-    <mergeCell ref="L83:M83"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L73:M73"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="L74:M74"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="L77:M77"/>
-    <mergeCell ref="L78:M78"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="N50:Q50"/>
-    <mergeCell ref="N51:Q51"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="N53:Q53"/>
-    <mergeCell ref="N54:Q54"/>
-    <mergeCell ref="N55:Q55"/>
-    <mergeCell ref="N56:Q56"/>
-    <mergeCell ref="N59:Q59"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="N47:Q47"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="L44:R44"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="N45:Q45"/>
-    <mergeCell ref="N46:Q46"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="F40:J40"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="N73:Q73"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="N69:Q69"/>
+    <mergeCell ref="N74:Q74"/>
+    <mergeCell ref="N75:Q75"/>
+    <mergeCell ref="N76:Q76"/>
+    <mergeCell ref="N82:Q82"/>
+    <mergeCell ref="N77:Q77"/>
+    <mergeCell ref="N78:Q78"/>
+    <mergeCell ref="N79:Q79"/>
+    <mergeCell ref="N80:Q80"/>
+    <mergeCell ref="N81:Q81"/>
     <mergeCell ref="N48:Q48"/>
     <mergeCell ref="N49:Q49"/>
     <mergeCell ref="N58:Q58"/>
@@ -9129,20 +9078,66 @@
     <mergeCell ref="N85:Q85"/>
     <mergeCell ref="N86:Q86"/>
     <mergeCell ref="N68:Q68"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="N47:Q47"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="L44:R44"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="N51:Q51"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="N53:Q53"/>
+    <mergeCell ref="N54:Q54"/>
+    <mergeCell ref="N55:Q55"/>
+    <mergeCell ref="N56:Q56"/>
+    <mergeCell ref="N59:Q59"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="N62:Q62"/>
     <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="N74:Q74"/>
-    <mergeCell ref="N75:Q75"/>
-    <mergeCell ref="N76:Q76"/>
-    <mergeCell ref="N82:Q82"/>
-    <mergeCell ref="N77:Q77"/>
-    <mergeCell ref="N78:Q78"/>
-    <mergeCell ref="N79:Q79"/>
-    <mergeCell ref="N80:Q80"/>
-    <mergeCell ref="N81:Q81"/>
-    <mergeCell ref="N73:Q73"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="N69:Q69"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="L82:M82"/>
+    <mergeCell ref="L83:M83"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="L74:M74"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="L77:M77"/>
+    <mergeCell ref="L78:M78"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="N83:Q83"/>
+    <mergeCell ref="N84:Q84"/>
+    <mergeCell ref="L92:M92"/>
+    <mergeCell ref="N92:Q92"/>
+    <mergeCell ref="N93:Q93"/>
+    <mergeCell ref="N94:Q94"/>
+    <mergeCell ref="N95:Q95"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="N87:Q87"/>
+    <mergeCell ref="N88:Q88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9156,7 +9151,7 @@
   </sheetPr>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
@@ -11883,58 +11878,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="282" t="s">
         <v>204</v>
       </c>
       <c r="B1" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="277" t="s">
+      <c r="C1" s="289" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="278"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
+      <c r="F1" s="290"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="291"/>
+      <c r="A2" s="283"/>
       <c r="B2" s="160" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="279" t="s">
+      <c r="C2" s="291" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="279"/>
-      <c r="E2" s="279"/>
-      <c r="F2" s="280"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
+      <c r="F2" s="292"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="291"/>
+      <c r="A3" s="283"/>
       <c r="B3" s="161" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="281" t="s">
+      <c r="C3" s="293" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="281"/>
-      <c r="E3" s="281"/>
-      <c r="F3" s="282"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="294"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="292"/>
+      <c r="A4" s="284"/>
       <c r="B4" s="163" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="283" t="s">
+      <c r="C4" s="295" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="283"/>
-      <c r="E4" s="283"/>
-      <c r="F4" s="284"/>
+      <c r="D4" s="295"/>
+      <c r="E4" s="295"/>
+      <c r="F4" s="296"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="293" t="s">
+      <c r="A7" s="285" t="s">
         <v>310</v>
       </c>
       <c r="B7" s="167" t="s">
@@ -11960,7 +11955,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="294"/>
+      <c r="A8" s="286"/>
       <c r="B8" s="165" t="s">
         <v>143</v>
       </c>
@@ -11987,7 +11982,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="294"/>
+      <c r="A9" s="286"/>
       <c r="B9" s="161" t="s">
         <v>228</v>
       </c>
@@ -12014,7 +12009,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="294"/>
+      <c r="A10" s="286"/>
       <c r="B10" s="161" t="s">
         <v>463</v>
       </c>
@@ -12041,7 +12036,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="295"/>
+      <c r="A11" s="287"/>
       <c r="B11" s="163" t="s">
         <v>229</v>
       </c>
@@ -12084,7 +12079,7 @@
       <c r="A14" s="183"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="285" t="s">
+      <c r="A15" s="278" t="s">
         <v>519</v>
       </c>
       <c r="B15" s="167" t="s">
@@ -12095,7 +12090,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="286"/>
+      <c r="A16" s="288"/>
       <c r="B16" s="186" t="s">
         <v>146</v>
       </c>
@@ -12104,7 +12099,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="286"/>
+      <c r="A17" s="288"/>
       <c r="B17" s="101" t="s">
         <v>147</v>
       </c>
@@ -12113,7 +12108,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="286"/>
+      <c r="A18" s="288"/>
       <c r="B18" s="101" t="s">
         <v>148</v>
       </c>
@@ -12122,7 +12117,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="286"/>
+      <c r="A19" s="288"/>
       <c r="B19" s="101" t="s">
         <v>149</v>
       </c>
@@ -12131,7 +12126,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="286"/>
+      <c r="A20" s="288"/>
       <c r="B20" s="101" t="s">
         <v>150</v>
       </c>
@@ -12141,7 +12136,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="286"/>
+      <c r="A21" s="288"/>
       <c r="B21" s="101" t="s">
         <v>151</v>
       </c>
@@ -12151,7 +12146,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="287"/>
+      <c r="A22" s="279"/>
       <c r="B22" s="102" t="s">
         <v>465</v>
       </c>
@@ -12162,7 +12157,7 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="285" t="s">
+      <c r="A26" s="278" t="s">
         <v>521</v>
       </c>
       <c r="B26" s="172"/>
@@ -12198,7 +12193,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="286"/>
+      <c r="A27" s="288"/>
       <c r="B27" s="197" t="s">
         <v>143</v>
       </c>
@@ -12233,7 +12228,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="286"/>
+      <c r="A28" s="288"/>
       <c r="B28" s="198" t="s">
         <v>228</v>
       </c>
@@ -12256,7 +12251,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="286"/>
+      <c r="A29" s="288"/>
       <c r="B29" s="198" t="s">
         <v>462</v>
       </c>
@@ -12281,7 +12276,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="286"/>
+      <c r="A30" s="288"/>
       <c r="B30" s="198" t="s">
         <v>229</v>
       </c>
@@ -12306,7 +12301,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="286"/>
+      <c r="A31" s="288"/>
       <c r="B31" s="198" t="s">
         <v>522</v>
       </c>
@@ -12352,7 +12347,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="286"/>
+      <c r="A32" s="288"/>
       <c r="B32" s="198" t="s">
         <v>523</v>
       </c>
@@ -12398,7 +12393,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="287"/>
+      <c r="A33" s="279"/>
       <c r="B33" s="199"/>
       <c r="C33" s="102"/>
       <c r="D33" s="62" t="s">
@@ -12418,21 +12413,21 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="285" t="s">
+      <c r="A36" s="278" t="s">
         <v>520</v>
       </c>
-      <c r="B36" s="245" t="s">
+      <c r="B36" s="268" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="288">
+      <c r="C36" s="280">
         <f>SUMPRODUCT(E8:E11*K27:K30)</f>
         <v>13837.053999999998</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="287"/>
-      <c r="B37" s="243"/>
-      <c r="C37" s="289"/>
+      <c r="A37" s="279"/>
+      <c r="B37" s="252"/>
+      <c r="C37" s="281"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="188"/>
@@ -12495,89 +12490,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="296" t="s">
+      <c r="A1" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="C1" s="297"/>
-      <c r="D1" s="298"/>
+      <c r="B1" s="298"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="299"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="302" t="s">
+      <c r="A2" s="303" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="307" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="308"/>
+      <c r="C2" s="308"/>
+      <c r="D2" s="309"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="303"/>
-      <c r="B3" s="309" t="s">
+      <c r="A3" s="304"/>
+      <c r="B3" s="310" t="s">
         <v>264</v>
       </c>
-      <c r="C3" s="310"/>
-      <c r="D3" s="311"/>
+      <c r="C3" s="311"/>
+      <c r="D3" s="312"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="303"/>
-      <c r="B4" s="309" t="s">
+      <c r="A4" s="304"/>
+      <c r="B4" s="310" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="310"/>
-      <c r="D4" s="311"/>
+      <c r="C4" s="311"/>
+      <c r="D4" s="312"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="200" t="s">
         <v>530</v>
       </c>
-      <c r="B5" s="249">
+      <c r="B5" s="242">
         <v>38.64</v>
       </c>
-      <c r="C5" s="250"/>
-      <c r="D5" s="304"/>
+      <c r="C5" s="243"/>
+      <c r="D5" s="305"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="200" t="s">
         <v>528</v>
       </c>
-      <c r="B6" s="249">
+      <c r="B6" s="242">
         <f>(24*2 + 7.5)*0.8+16+14</f>
         <v>74.400000000000006</v>
       </c>
-      <c r="C6" s="250"/>
-      <c r="D6" s="304"/>
+      <c r="C6" s="243"/>
+      <c r="D6" s="305"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="200" t="s">
         <v>529</v>
       </c>
-      <c r="B7" s="249">
+      <c r="B7" s="242">
         <f>B6*B5</f>
         <v>2874.8160000000003</v>
       </c>
-      <c r="C7" s="250"/>
-      <c r="D7" s="304"/>
+      <c r="C7" s="243"/>
+      <c r="D7" s="305"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="201" t="s">
         <v>531</v>
       </c>
-      <c r="B8" s="243">
+      <c r="B8" s="252">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="C8" s="264"/>
-      <c r="D8" s="305"/>
+      <c r="C8" s="253"/>
+      <c r="D8" s="306"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="299" t="s">
+      <c r="A10" s="300" t="s">
         <v>526</v>
       </c>
-      <c r="B10" s="300"/>
-      <c r="C10" s="300"/>
-      <c r="D10" s="301"/>
+      <c r="B10" s="301"/>
+      <c r="C10" s="301"/>
+      <c r="D10" s="302"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="165"/>
@@ -12851,7 +12846,7 @@
       <c r="F13" s="214"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="312" t="s">
+      <c r="A14" s="313" t="s">
         <v>126</v>
       </c>
       <c r="B14" s="101" t="s">
@@ -12870,7 +12865,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="313"/>
+      <c r="A15" s="314"/>
       <c r="B15" s="101" t="s">
         <v>130</v>
       </c>
@@ -12887,7 +12882,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="313"/>
+      <c r="A16" s="314"/>
       <c r="B16" s="101" t="s">
         <v>132</v>
       </c>
@@ -12904,7 +12899,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="314"/>
+      <c r="A17" s="315"/>
       <c r="B17" s="101" t="s">
         <v>134</v>
       </c>
@@ -12921,7 +12916,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="312" t="s">
+      <c r="A18" s="313" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="101" t="s">
@@ -12940,7 +12935,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="314"/>
+      <c r="A19" s="315"/>
       <c r="B19" s="205" t="s">
         <v>195</v>
       </c>
@@ -13112,7 +13107,7 @@
       <c r="F2" s="218"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="315" t="s">
+      <c r="A3" s="316" t="s">
         <v>537</v>
       </c>
       <c r="B3" s="100" t="s">
@@ -13133,7 +13128,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="316"/>
+      <c r="A4" s="317"/>
       <c r="B4" s="102" t="s">
         <v>94</v>
       </c>
@@ -13154,7 +13149,7 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="315" t="s">
+      <c r="A6" s="316" t="s">
         <v>538</v>
       </c>
       <c r="B6" s="100" t="s">
@@ -13173,7 +13168,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="317"/>
+      <c r="A7" s="318"/>
       <c r="B7" s="101" t="s">
         <v>161</v>
       </c>
@@ -13190,7 +13185,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="317"/>
+      <c r="A8" s="318"/>
       <c r="B8" s="101" t="s">
         <v>164</v>
       </c>
@@ -13207,7 +13202,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="317"/>
+      <c r="A9" s="318"/>
       <c r="B9" s="101" t="s">
         <v>185</v>
       </c>
@@ -13221,7 +13216,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="316"/>
+      <c r="A10" s="317"/>
       <c r="B10" s="102" t="s">
         <v>187</v>
       </c>
@@ -13240,7 +13235,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="315" t="s">
+      <c r="A12" s="316" t="s">
         <v>539</v>
       </c>
       <c r="B12" s="100" t="s">
@@ -13259,7 +13254,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="317"/>
+      <c r="A13" s="318"/>
       <c r="B13" s="101" t="s">
         <v>158</v>
       </c>
@@ -13276,7 +13271,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="316"/>
+      <c r="A14" s="317"/>
       <c r="B14" s="102" t="s">
         <v>173</v>
       </c>
@@ -13298,7 +13293,7 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="315" t="s">
+      <c r="A16" s="316" t="s">
         <v>540</v>
       </c>
       <c r="B16" s="100" t="s">
@@ -13317,7 +13312,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="317"/>
+      <c r="A17" s="318"/>
       <c r="B17" s="101" t="s">
         <v>168</v>
       </c>
@@ -13334,7 +13329,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="317"/>
+      <c r="A18" s="318"/>
       <c r="B18" s="101" t="s">
         <v>169</v>
       </c>
@@ -13351,7 +13346,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="316"/>
+      <c r="A19" s="317"/>
       <c r="B19" s="102" t="s">
         <v>171</v>
       </c>
@@ -13392,7 +13387,7 @@
       <c r="A22" s="185"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="315" t="s">
+      <c r="A23" s="316" t="s">
         <v>542</v>
       </c>
       <c r="B23" s="100" t="s">
@@ -13408,7 +13403,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="316"/>
+      <c r="A24" s="317"/>
       <c r="B24" s="102" t="s">
         <v>278</v>
       </c>
@@ -13642,7 +13637,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="315" t="s">
+      <c r="A3" s="316" t="s">
         <v>546</v>
       </c>
       <c r="B3" s="100" t="s">
@@ -13663,7 +13658,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="317"/>
+      <c r="A4" s="318"/>
       <c r="B4" s="101" t="s">
         <v>86</v>
       </c>
@@ -13682,7 +13677,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="317"/>
+      <c r="A5" s="318"/>
       <c r="B5" s="101" t="s">
         <v>91</v>
       </c>
@@ -13701,7 +13696,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="317"/>
+      <c r="A6" s="318"/>
       <c r="B6" s="101" t="s">
         <v>355</v>
       </c>
@@ -13720,7 +13715,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="317"/>
+      <c r="A7" s="318"/>
       <c r="B7" s="101" t="s">
         <v>384</v>
       </c>
@@ -13736,7 +13731,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="317"/>
+      <c r="A8" s="318"/>
       <c r="B8" s="101" t="s">
         <v>382</v>
       </c>
@@ -13752,7 +13747,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="316"/>
+      <c r="A9" s="317"/>
       <c r="B9" s="102" t="s">
         <v>387</v>
       </c>
@@ -13772,7 +13767,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="315" t="s">
+      <c r="A11" s="316" t="s">
         <v>547</v>
       </c>
       <c r="B11" s="100" t="s">
@@ -13792,7 +13787,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="316"/>
+      <c r="A12" s="317"/>
       <c r="B12" s="102" t="s">
         <v>222</v>
       </c>
@@ -13839,7 +13834,7 @@
       <c r="A15" s="185"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="315" t="s">
+      <c r="A16" s="316" t="s">
         <v>548</v>
       </c>
       <c r="B16" s="100" t="s">
@@ -13859,7 +13854,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="317"/>
+      <c r="A17" s="318"/>
       <c r="B17" s="101" t="s">
         <v>361</v>
       </c>
@@ -13877,7 +13872,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="317"/>
+      <c r="A18" s="318"/>
       <c r="B18" s="101" t="s">
         <v>363</v>
       </c>
@@ -13895,7 +13890,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="317"/>
+      <c r="A19" s="318"/>
       <c r="B19" s="101" t="s">
         <v>365</v>
       </c>
@@ -13913,7 +13908,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="317"/>
+      <c r="A20" s="318"/>
       <c r="B20" s="101" t="s">
         <v>367</v>
       </c>
@@ -13931,7 +13926,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="317"/>
+      <c r="A21" s="318"/>
       <c r="B21" s="101" t="s">
         <v>370</v>
       </c>
@@ -13949,7 +13944,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="317"/>
+      <c r="A22" s="318"/>
       <c r="B22" s="101" t="s">
         <v>296</v>
       </c>
@@ -13965,7 +13960,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="317"/>
+      <c r="A23" s="318"/>
       <c r="B23" s="101" t="s">
         <v>294</v>
       </c>
@@ -13981,7 +13976,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="316"/>
+      <c r="A24" s="317"/>
       <c r="B24" s="102" t="s">
         <v>357</v>
       </c>
@@ -14002,7 +13997,7 @@
       <c r="A25" s="185"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="315" t="s">
+      <c r="A26" s="316" t="s">
         <v>549</v>
       </c>
       <c r="B26" s="100" t="s">
@@ -14022,7 +14017,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="316"/>
+      <c r="A27" s="317"/>
       <c r="B27" s="102" t="s">
         <v>482</v>
       </c>

</xml_diff>